<commit_message>
New air dehumidification set
</commit_message>
<xml_diff>
--- a/PRC.xlsx
+++ b/PRC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61693\Desktop\Panasonic\project_oct\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86165C9A-9F0B-4C6C-AE6E-E51E91CFA9A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D494DD61-3B8E-4F46-9B34-BAFC7C4F7FF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3110" yWindow="1230" windowWidth="16920" windowHeight="10640" xr2:uid="{2CFB3B8B-50E1-4174-969D-63782635CD2B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" xr2:uid="{2CFB3B8B-50E1-4174-969D-63782635CD2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
   <si>
     <t>Minimum Filter Efficiency(ab)</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>School Classrooms</t>
-  </si>
-  <si>
-    <t>Apartment Building</t>
   </si>
   <si>
     <t>Doctor Office</t>
@@ -164,6 +161,12 @@
   <si>
     <t>Minimum 
 outdoor ach</t>
+  </si>
+  <si>
+    <t>Multifamily Housing</t>
+  </si>
+  <si>
+    <t>—</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F12" sqref="F12:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,25 +547,25 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -570,22 +573,25 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
+      <c r="H2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -599,16 +605,19 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
+      <c r="H3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -619,55 +628,157 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -676,47 +787,50 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -725,44 +839,50 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
         <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -771,21 +891,24 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -794,13 +917,16 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>